<commit_message>
Finished and revised first part of five steps to complete.
</commit_message>
<xml_diff>
--- a/V Cycle Process/V_Cycle Process Script.xlsx
+++ b/V Cycle Process/V_Cycle Process Script.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="1"/>
   </bookViews>
@@ -525,6 +525,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -532,12 +538,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1989,9 +1989,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2003,10 +2006,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="C2:E33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,7 +2045,7 @@
       </c>
     </row>
     <row r="9" spans="3:5" s="13" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="49" t="s">
         <v>99</v>
       </c>
       <c r="D9" s="38" t="s">
@@ -2049,13 +2053,13 @@
       </c>
     </row>
     <row r="10" spans="3:5" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="52"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="53"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="40" t="s">
         <v>20</v>
       </c>
@@ -2072,10 +2076,10 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="49">
+      <c r="C14" s="51">
         <v>1</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="52" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -2083,31 +2087,31 @@
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="27" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="29" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="49">
+      <c r="C18" s="51">
         <v>2</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="52" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -2115,36 +2119,36 @@
       </c>
     </row>
     <row r="19" spans="3:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="27" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="27" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="5"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="49">
+      <c r="C23" s="51">
         <v>3</v>
       </c>
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="52" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="22" t="s">
@@ -2152,22 +2156,22 @@
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
       <c r="E24" s="33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="27" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
       <c r="E26" s="24" t="s">
         <v>23</v>
       </c>
@@ -2230,10 +2234,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="C2:E27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,10 +2308,10 @@
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="49">
+      <c r="C15" s="51">
         <v>1</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="52" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -2314,31 +2319,31 @@
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="27" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="49">
+      <c r="C19" s="51">
         <v>2</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="52" t="s">
         <v>88</v>
       </c>
       <c r="E19" s="22" t="s">
@@ -2346,20 +2351,20 @@
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="28" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="5"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
@@ -2407,6 +2412,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="C2:E31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2482,10 +2488,10 @@
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="49">
+      <c r="C15" s="51">
         <v>1</v>
       </c>
-      <c r="D15" s="50" t="s">
+      <c r="D15" s="52" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="22" t="s">
@@ -2493,29 +2499,29 @@
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="27" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="49"/>
-      <c r="D17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
       <c r="E17" s="28" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="49">
+      <c r="C19" s="51">
         <v>2</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="52" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="35" t="s">
@@ -2523,29 +2529,29 @@
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="27" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
       <c r="E22" s="24"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="49">
+      <c r="C23" s="51">
         <v>3</v>
       </c>
-      <c r="D23" s="50" t="s">
+      <c r="D23" s="52" t="s">
         <v>39</v>
       </c>
       <c r="E23" s="35" t="s">
@@ -2553,22 +2559,22 @@
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
       <c r="E24" s="35" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="52"/>
       <c r="E25" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
       <c r="E26" s="24"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
@@ -2621,6 +2627,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="C2:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -2684,10 +2691,10 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="49">
+      <c r="C13" s="51">
         <v>1</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="52" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="36" t="s">
@@ -2695,29 +2702,29 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="43" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="49">
+      <c r="C17" s="51">
         <v>2</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="52" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="36" t="s">
@@ -2725,22 +2732,22 @@
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="27" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="42" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="29"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
@@ -2788,10 +2795,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="C2:E32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2851,10 +2859,10 @@
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="49">
+      <c r="C13" s="51">
         <v>1</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="52" t="s">
         <v>48</v>
       </c>
       <c r="E13" s="36" t="s">
@@ -2862,29 +2870,29 @@
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="49"/>
-      <c r="D14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
       <c r="E14" s="43" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
       <c r="E15" s="28" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="49">
+      <c r="C17" s="51">
         <v>2</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="52" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="36" t="s">
@@ -2892,22 +2900,22 @@
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="49"/>
-      <c r="D18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
       <c r="E18" s="27" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C19" s="49"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
       <c r="E19" s="42" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
       <c r="E20" s="29"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
@@ -2946,8 +2954,8 @@
       <c r="D28" s="37"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="51"/>
-      <c r="D29" s="50" t="s">
+      <c r="C29" s="53"/>
+      <c r="D29" s="52" t="s">
         <v>85</v>
       </c>
       <c r="E29" s="36" t="s">
@@ -2955,22 +2963,22 @@
       </c>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" s="51"/>
-      <c r="D30" s="50"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="52"/>
       <c r="E30" s="27" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C31" s="51"/>
-      <c r="D31" s="50"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="42" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="32" spans="3:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="C32" s="51"/>
-      <c r="D32" s="50"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="52"/>
       <c r="E32" s="41" t="s">
         <v>86</v>
       </c>

</xml_diff>